<commit_message>
Update Estadísticas normales Datos abiertos 1991-2020 - AJUSTADO.xlsx
</commit_message>
<xml_diff>
--- a/Entregas_Parcial/datos/Estadísticas normales Datos abiertos 1991-2020 - AJUSTADO.xlsx
+++ b/Entregas_Parcial/datos/Estadísticas normales Datos abiertos 1991-2020 - AJUSTADO.xlsx
@@ -390,7 +390,7 @@
     <t>HELADAS</t>
   </si>
   <si>
-    <t>OBJETIVO</t>
+    <t>Objetivo</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1201,7 @@
   <dimension ref="A1:L1172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>